<commit_message>
Update with total cost
</commit_message>
<xml_diff>
--- a/Spring19/Parts List.xlsx
+++ b/Spring19/Parts List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepthinacharaju/Desktop/MediCall/Spring19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB0E2C4A-F46F-7F48-B271-EEC02A418957}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B10C41C-C612-9C4C-9CAB-0299854AC017}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16640" xr2:uid="{800F3859-DB4D-784B-A23A-9EED9A7713DD}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Part</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Relay on Mantech</t>
+  </si>
+  <si>
+    <t>Total Cost:</t>
   </si>
 </sst>
 </file>
@@ -180,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,8 +196,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7E79"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -217,12 +226,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,6 +276,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -248,6 +293,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7E79"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -556,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741C83BD-39F9-7046-972B-200F1345A55D}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -805,30 +855,45 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:8" ht="17" thickBot="1">
+      <c r="A10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="15">
         <v>20.88</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="15">
         <v>20.88</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="16">
         <v>1</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="15">
         <f>E10*D10</f>
         <v>20.88</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="19">
+        <f>SUM(F2:F10)</f>
+        <v>58.432333333333332</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>